<commit_message>
add DQ indicators for Orpha coding
</commit_message>
<xml_diff>
--- a/Data/medData/dqTestData_KT.xlsx
+++ b/Data/medData/dqTestData_KT.xlsx
@@ -356,10 +356,10 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
@@ -709,7 +709,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>321</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>